<commit_message>
updates to AI MSE startups
updates from Andy Soder
</commit_message>
<xml_diff>
--- a/course_notes/AI_MSE_companies_Jan2026_nonexhaustive.xlsx
+++ b/course_notes/AI_MSE_companies_Jan2026_nonexhaustive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\teaching\5540-6640 Materials Informatics\MaterialsInformatics\course_notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansoan/Documents/Materiale_Kemi/Company/Company_Nano-SDL/Competitors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90426C0-4EC5-408B-8C6D-DCA249AFD00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CE5B038-F803-3E43-8D54-46CEEFF8823A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3260" yWindow="-20980" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="225">
   <si>
     <t>company</t>
   </si>
@@ -100,9 +100,6 @@
     <t>https://www.cusp.ai/</t>
   </si>
   <si>
-    <t>$30M seed (Jun 2024)</t>
-  </si>
-  <si>
     <t>Cambridge team incl. academic founders (per coverage; details on site)</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>https://www.kebotix.com/</t>
   </si>
   <si>
-    <t>$11.4M Series A announced (Jan 2020)</t>
-  </si>
-  <si>
     <t>(AI-powered self-driving lab; academic founders not in sources)</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
     <t>Autonomous discovery platform</t>
   </si>
   <si>
-    <t>https://www.kebotix.com/news/kebotix-raises-114-million-in-series-a-funding-for-rapid-discovery-of-chemicals-materials-to-address-global-challenges</t>
-  </si>
-  <si>
     <t>NobleAI</t>
   </si>
   <si>
@@ -493,9 +484,6 @@
     <t>https://www.materialsnexus.com/</t>
   </si>
   <si>
-    <t>£2.08M seed (Jul 2023)</t>
-  </si>
-  <si>
     <t>Jonathan Bean (founder; physicist at University of Cambridge)</t>
   </si>
   <si>
@@ -505,9 +493,6 @@
     <t>Materials discovery platform for sustainable substitutes</t>
   </si>
   <si>
-    <t>https://www.uktechnews.info/2023/07/26/materials-nexus-secures-2-08-million-investment-led-by-ada-ventures/ ; https://medium.com/ada-ventures/materials-nexus-why-ada-ventures-invested-b06b45b71b2a</t>
-  </si>
-  <si>
     <t>PhaseTree</t>
   </si>
   <si>
@@ -680,13 +665,43 @@
   </si>
   <si>
     <t>NOTE! This is definitely a non-exhaustive list. It was assembled January 2026.  Compiled for teaching purposes; funding amounts from public sources and databases; not an investment analysis</t>
+  </si>
+  <si>
+    <t>$30M seed (Jun 2024) $100M seed (2025)</t>
+  </si>
+  <si>
+    <t>Entalpic</t>
+  </si>
+  <si>
+    <t>$11.4M Series A announced (Jan 2020) $2.2M Series A (2023) $5 Series B (2024)</t>
+  </si>
+  <si>
+    <t>https://www.kebotix.com/news/kebotix-raises-114-million-in-series-a-funding-for-rapid-discovery-of-chemicals-materials-to-address-global-challenges &amp; https://tracxn.com/d/companies/kebotix/__TJFXLOaaexuBKLHzYyy3ozL5BXWE7J_jv5Iu4DMVm7c/funding-and-investors#funding-rounds</t>
+  </si>
+  <si>
+    <t>$8.5M seed (2024)</t>
+  </si>
+  <si>
+    <t>https://entalpic.ai/</t>
+  </si>
+  <si>
+    <t>Generative AI platform for discovery and co-develop strong IP for costumer.</t>
+  </si>
+  <si>
+    <t>Alexandre Duval</t>
+  </si>
+  <si>
+    <t>https://www.uktechnews.info/2023/07/26/materials-nexus-secures-2-08-million-investment-led-by-ada-ventures/ ; https://medium.com/ada-ventures/materials-nexus-why-ada-ventures-invested-b06b45b71b2a &amp; https://climateinnovation.impactmap.cam.ac.uk/matnex/</t>
+  </si>
+  <si>
+    <t>£2.08M seed (Jul 2023), disclosed in talk at AIS25: £15M in 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,6 +738,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -745,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -756,6 +778,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1091,11 +1116,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="173" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -1105,12 +1132,12 @@
     <col min="7" max="7" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1130,11 +1157,11 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1145,7 +1172,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -1157,7 +1184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1193,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -1178,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1228,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1209,628 +1236,648 @@
         <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G34" t="s">
         <v>211</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B33" t="s">
-        <v>207</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E33" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G34" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data access examples NOMAD
</commit_message>
<xml_diff>
--- a/course_notes/AI_MSE_companies_Jan2026_nonexhaustive.xlsx
+++ b/course_notes/AI_MSE_companies_Jan2026_nonexhaustive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansoan/Documents/Materiale_Kemi/Company/Company_Nano-SDL/Competitors/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\teaching\5540-6640 Materials Informatics\MaterialsInformatics\course_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CE5B038-F803-3E43-8D54-46CEEFF8823A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE477E80-7E78-4416-A0C9-B92C73670CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3260" yWindow="-20980" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="234">
   <si>
     <t>company</t>
   </si>
@@ -695,6 +695,33 @@
   </si>
   <si>
     <t>£2.08M seed (Jul 2023), disclosed in talk at AIS25: £15M in 2025</t>
+  </si>
+  <si>
+    <t>Project Prometheus</t>
+  </si>
+  <si>
+    <t>$6.2B from Bezos fund</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2025/11/17/technology/bezos-project-prometheus.html</t>
+  </si>
+  <si>
+    <t>Jeff Bezos backing, Vik Bajaj (formerly Google X, Verily, Foresite Labs)</t>
+  </si>
+  <si>
+    <t>https://en.xtalpi.com/</t>
+  </si>
+  <si>
+    <t>XtalPi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug discovery, lithium-sulfur batteries, </t>
+  </si>
+  <si>
+    <t>https://www.texau.com/profiles/xtal-pi</t>
+  </si>
+  <si>
+    <t>$784M ($400 million in Series D (August 11, 2021), $268 million in Post-IPO (February 27, 2025), and $ 116 million in Post-IPO (September 17, 2025).)</t>
   </si>
 </sst>
 </file>
@@ -1116,13 +1143,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="173" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="173" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -1132,12 +1159,12 @@
     <col min="7" max="7" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1188,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1228,7 +1255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1251,7 +1278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1274,7 +1301,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1297,7 +1324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -1320,7 +1347,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1343,7 +1370,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
@@ -1366,7 +1393,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>64</v>
       </c>
@@ -1389,7 +1416,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>71</v>
       </c>
@@ -1412,7 +1439,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>78</v>
       </c>
@@ -1435,7 +1462,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1458,7 +1485,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>90</v>
       </c>
@@ -1481,7 +1508,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>97</v>
       </c>
@@ -1504,7 +1531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>104</v>
       </c>
@@ -1527,7 +1554,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>111</v>
       </c>
@@ -1550,7 +1577,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>118</v>
       </c>
@@ -1573,7 +1600,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>124</v>
       </c>
@@ -1596,7 +1623,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>131</v>
       </c>
@@ -1619,7 +1646,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>138</v>
       </c>
@@ -1642,7 +1669,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>145</v>
       </c>
@@ -1665,7 +1692,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>152</v>
       </c>
@@ -1688,7 +1715,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>157</v>
       </c>
@@ -1711,7 +1738,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>164</v>
       </c>
@@ -1734,7 +1761,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>171</v>
       </c>
@@ -1757,7 +1784,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>178</v>
       </c>
@@ -1780,7 +1807,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>185</v>
       </c>
@@ -1803,7 +1830,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>191</v>
       </c>
@@ -1826,7 +1853,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>201</v>
       </c>
@@ -1840,7 +1867,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>208</v>
       </c>
@@ -1860,7 +1887,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>216</v>
       </c>
@@ -1878,6 +1905,37 @@
       </c>
       <c r="F35" s="6" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" t="s">
+        <v>233</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G37" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>